<commit_message>
Got the new architecture scaffolded. Time to implement.
</commit_message>
<xml_diff>
--- a/WorkBot/refactor/data/orders/Webstaurant/Webstaurant_Bakery_2025-08-30.xlsx
+++ b/WorkBot/refactor/data/orders/Webstaurant/Webstaurant_Bakery_2025-08-30.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1011,6 +1011,60 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>150300865</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bag Paper - 6x13.5 Window</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>79.99</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>319.96</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>588MILK632</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Urnex - Rinza</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>17.99</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>431.76</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>